<commit_message>
Finalizado página de softwares disponíveis
</commit_message>
<xml_diff>
--- a/arquivos_bd/LEVANTAMENTO DE SOFTWARES LAB INFO.xlsx
+++ b/arquivos_bd/LEVANTAMENTO DE SOFTWARES LAB INFO.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projeto_estagio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projeto_estagio\arquivos_bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Microsoft" sheetId="2" r:id="rId2"/>
     <sheet name="INSERT" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>Android Studio</t>
   </si>
@@ -211,16 +211,64 @@
     <t>local_software</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
-    <t>INSERT INTO softwares_disponiveis (nome_software, descricao_software, local) values(</t>
+    <t>NOME_ARQUIVO</t>
+  </si>
+  <si>
+    <t>NOME_IMAGEM</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values(</t>
+  </si>
+  <si>
+    <t>android-studio-bundle-135.1641136.exe</t>
+  </si>
+  <si>
+    <t>android-studio.jpg</t>
+  </si>
+  <si>
+    <t>CÓDIGO_SQL</t>
+  </si>
+  <si>
+    <t>astah-community-6_8_0-d254c5-jre-setup</t>
+  </si>
+  <si>
+    <t>astah.png</t>
+  </si>
+  <si>
+    <t>case_studio.gif</t>
+  </si>
+  <si>
+    <t>CS2_setup.exe</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>packettracer533</t>
+  </si>
+  <si>
+    <t>packet_tracer.jpg</t>
+  </si>
+  <si>
+    <t>Dev-Cpp 64 bits</t>
+  </si>
+  <si>
+    <t>dev_c++.jpg</t>
+  </si>
+  <si>
+    <t>dia.jpg</t>
+  </si>
+  <si>
+    <t>dia-setup-0.97.2-2.exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,7 +338,18 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -869,297 +928,511 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>UPPER("local_software")</f>
-        <v>LOCAL_SOFTWARE</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="str">
+        <f>CONCATENATE($A$1,"'",B3,"'",", ","'",C3,"'",", ", "'",D3,"'",", ", "'",E3,"'",");")</f>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Android Studio', 'Android Studio é um ambiente de desenvolvimento integrado para desenvolver para a plataforma Android. ', 'android-studio-bundle-135.1641136.exe', 'android-studio.jpg');</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F24" si="0">CONCATENATE($A$1,"'",B4,"'",", ","'",C4,"'",", ", "'",D4,"'",", ", "'",E4,"'",");")</f>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Astah', 'IDE para Modelagem de Dados (UML) criada com Java e de uso fácil e intuitivo.', 'astah-community-6_8_0-d254c5-jre-setup', 'astah.png');</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Case Studio', 'Ferramenta para modelagem de dados.', 'CS2_setup.exe', 'case_studio.gif');</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Cisco Packet Tracer', 'O Packet Tracer é um programa educacional gratuito que permite simular uma rede de computadores, através de equipamentos e configurações presente em situações reais.', 'packettracer533', 'packet_tracer.jpg');</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" t="str">
-        <f>CONCATENATE("'",B7,"'")</f>
-        <v>'Android Studio'</v>
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE("'",C7,"'")</f>
-        <v>'Android Studio é um ambiente de desenvolvimento integrado para desenvolver para a plataforma Android. '</v>
-      </c>
-      <c r="G7" t="str">
-        <f>CONCATENATE("'",D7,"'")</f>
-        <v>'local'</v>
-      </c>
-      <c r="H7" t="str">
-        <f>CONCATENATE(A1,E7,", ",F7,", ", G7,");")</f>
-        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, local) values('Android Studio', 'Android Studio é um ambiente de desenvolvimento integrado para desenvolver para a plataforma Android. ', 'local');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Dev C++', 'Linguagem de programação de alto nível com facilidades para o uso em baixo nível, multiparadigma e de uso geral.', 'Dev-Cpp 64 bits', 'dev_c++.jpg');</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Dia', 'Dia é uma aplicação gratuita/freeware para desenho de diagramas.', 'dia-setup-0.97.2-2.exe', 'dia.jpg');</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Easy PHP', 'Programa que instala em apenas um passo o servidor Apache, junto com o módulo para programação em PHP e o banco de dados MySQL.', '-', '-');</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Eclipse', 'Ambiente de desenvolvimento integrado (IDE) gratuito e de código aberto usado para o desenvolvimento de software com a linguagem Java.', '-', '-');</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Erwin Data Modeler', 'O CA ERwin Data Modeler, normalmente referido apenas por Erwin, é uma ferramenta de software utilizada para a modelação de sistemas de informação.', '-', '-');</v>
+      </c>
+      <c r="G11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Firebird', 'Sistema gerenciador de banco de dados. Roda em Linux, Windows, Mac OS e uma variedade de plataformas Unix', '-', '-');</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Geny Motion', 'Emulador para testes de aplicações android.', '-', '-');</v>
+      </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('HTML Kit', 'Editor HTML.', '-', '-');</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('MySQL', 'Sistema de gerenciamento de banco de dados (SGBD), que utiliza a linguagem SQL (Linguagem de Consulta Estruturada, do inglês Structured Query Language) como interface.', '-', '-');</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Netbeans', 'Ambiente de desenvolvimento integrado (IDE) gratuito e de código aberto usado para o desenvolvimento de software com as linguagens Java, C/C++, PHP, Python, entre outras.', '-', '-');</v>
+      </c>
+      <c r="G16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Notepad ++', 'Editor de texto rico em funções, desenvolvido para ajudar autores de scripts, HTMLs e XMLs à editar, formatar, validar, visualizar e publicar páginas na Web.', '-', '-');</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('SQL Yog', 'SQLyog é um programa desenvolvido pela WEByog Enterprise que possibilita a edição de bancos de dados Mysql, que baseados na linguagem SQL. Utilizado na criação, edição, sincronização de banco de dados internos e em servidores.', '-', '-');</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Sublime text', 'Software multiplataforma de edição de texto, no entanto utilizado por muitos desenvolvedores para editar código-fonte, escrito em linguagem Python', '-', '-');</v>
+      </c>
+      <c r="G19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Ubuntu - Linux', 'Distribuição do sistema operacional Linux baseado na distribuição Debian, sendo uma das distribuições mais populares.', '-', '-');</v>
+      </c>
+      <c r="G20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Unity', 'Unity, também conhecido como Unity 3D, é um motor de jogo 3D proprietário e uma IDE criado pela Unity Technologies.', '-', '-');</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Virtual Box', 'Software de virtualização desenvolvido pela Sun Microsystems que, como o VMware Workstation, visa criar ambientes para instalação de sistemas distintos. Ele permite a instalação e utilização de um sistema operativo dentro de outro dando suporte real a softwares de outros sistemas.', '-', '-');</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('VisualG', 'IDE que edita, interpreta e executa algoritmos com uma linguagem próxima do portugues estruturado, como um programa normal de computador. Com recurso para executar algoritmos e visualizador de variáveis que funciona como um depurador.', '-', '-');</v>
+      </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO softwares_disponiveis (nome_software, descricao_software, nome_arquivo, nome_imagem) values('Xampp', 'Servidor independente de plataforma, software livre, que consiste principalmente na base de dados MySQL, o servidor web Apache e os interpretadores para linguagens de script: PHP e Perl.', '-', '-');</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G3:G24">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criada nova página: tabela_softwares
</commit_message>
<xml_diff>
--- a/arquivos_bd/LEVANTAMENTO DE SOFTWARES LAB INFO.xlsx
+++ b/arquivos_bd/LEVANTAMENTO DE SOFTWARES LAB INFO.xlsx
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>